<commit_message>
Added Test Updation API
</commit_message>
<xml_diff>
--- a/server/uploads/test.xlsx
+++ b/server/uploads/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Question</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,6 +436,26 @@
       </c>
       <c r="F2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>